<commit_message>
refactored timbre and rhythm decomposition approach
</commit_message>
<xml_diff>
--- a/timbre_and_rhythm_features_decomposition/recommendations_for_tracks.xlsx
+++ b/timbre_and_rhythm_features_decomposition/recommendations_for_tracks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="102">
   <si>
     <t>01 - Paper Gods.csv</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>21. Cantamus - Aurora.csv</t>
+  </si>
+  <si>
+    <t>Ludovico Einaudi – Una Mattina.csv</t>
   </si>
   <si>
     <t>morricone_30s.csv</t>
@@ -674,13 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW21"/>
+  <dimension ref="A1:CX21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:101">
+    <row r="1" spans="1:102">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,8 +987,11 @@
       <c r="CW1" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="CX1" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="2" spans="1:101">
+    <row r="2" spans="1:102">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1289,8 +1295,11 @@
       <c r="CW2" t="s">
         <v>100</v>
       </c>
+      <c r="CX2" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="3" spans="1:101">
+    <row r="3" spans="1:102">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>76</v>
       </c>
       <c r="U3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="V3" t="s">
         <v>63</v>
@@ -1517,7 +1526,7 @@
         <v>47</v>
       </c>
       <c r="BX3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BY3" t="s">
         <v>0</v>
@@ -1589,13 +1598,16 @@
         <v>84</v>
       </c>
       <c r="CV3" t="s">
+        <v>20</v>
+      </c>
+      <c r="CW3" t="s">
         <v>75</v>
       </c>
-      <c r="CW3" t="s">
+      <c r="CX3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:101">
+    <row r="4" spans="1:102">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1657,7 +1669,7 @@
         <v>45</v>
       </c>
       <c r="U4" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="V4" t="s">
         <v>96</v>
@@ -1726,7 +1738,7 @@
         <v>71</v>
       </c>
       <c r="AR4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AS4" t="s">
         <v>9</v>
@@ -1735,7 +1747,7 @@
         <v>51</v>
       </c>
       <c r="AU4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AV4" t="s">
         <v>4</v>
@@ -1894,13 +1906,16 @@
         <v>70</v>
       </c>
       <c r="CV4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CW4" t="s">
         <v>52</v>
       </c>
-      <c r="CW4" t="s">
+      <c r="CX4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:101">
+    <row r="5" spans="1:102">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1962,7 +1977,7 @@
         <v>86</v>
       </c>
       <c r="U5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V5" t="s">
         <v>91</v>
@@ -1977,7 +1992,7 @@
         <v>48</v>
       </c>
       <c r="Z5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA5" t="s">
         <v>69</v>
@@ -2154,7 +2169,7 @@
         <v>4</v>
       </c>
       <c r="CG5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="CH5" t="s">
         <v>9</v>
@@ -2199,13 +2214,16 @@
         <v>20</v>
       </c>
       <c r="CV5" t="s">
+        <v>70</v>
+      </c>
+      <c r="CW5" t="s">
         <v>3</v>
       </c>
-      <c r="CW5" t="s">
+      <c r="CX5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:101">
+    <row r="6" spans="1:102">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2267,7 +2285,7 @@
         <v>37</v>
       </c>
       <c r="U6" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="V6" t="s">
         <v>52</v>
@@ -2282,7 +2300,7 @@
         <v>54</v>
       </c>
       <c r="Z6" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="AA6" t="s">
         <v>30</v>
@@ -2501,16 +2519,19 @@
         <v>94</v>
       </c>
       <c r="CU6" t="s">
+        <v>99</v>
+      </c>
+      <c r="CV6" t="s">
         <v>25</v>
       </c>
-      <c r="CV6" t="s">
+      <c r="CW6" t="s">
         <v>33</v>
       </c>
-      <c r="CW6" t="s">
+      <c r="CX6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:101">
+    <row r="7" spans="1:102">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2572,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="V7" t="s">
         <v>68</v>
@@ -2587,7 +2608,7 @@
         <v>27</v>
       </c>
       <c r="Z7" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="AA7" t="s">
         <v>65</v>
@@ -2722,7 +2743,7 @@
         <v>49</v>
       </c>
       <c r="BS7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BT7" t="s">
         <v>6</v>
@@ -2782,7 +2803,7 @@
         <v>93</v>
       </c>
       <c r="CM7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="CN7" t="s">
         <v>29</v>
@@ -2806,16 +2827,19 @@
         <v>20</v>
       </c>
       <c r="CU7" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="CV7" t="s">
+        <v>89</v>
+      </c>
+      <c r="CW7" t="s">
         <v>79</v>
       </c>
-      <c r="CW7" t="s">
+      <c r="CX7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:101">
+    <row r="8" spans="1:102">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -2826,7 +2850,7 @@
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
         <v>74</v>
@@ -2877,7 +2901,7 @@
         <v>7</v>
       </c>
       <c r="U8" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="V8" t="s">
         <v>53</v>
@@ -2892,7 +2916,7 @@
         <v>23</v>
       </c>
       <c r="Z8" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="AA8" t="s">
         <v>49</v>
@@ -3027,7 +3051,7 @@
         <v>67</v>
       </c>
       <c r="BS8" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="BT8" t="s">
         <v>24</v>
@@ -3111,16 +3135,19 @@
         <v>53</v>
       </c>
       <c r="CU8" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="CV8" t="s">
+        <v>92</v>
+      </c>
+      <c r="CW8" t="s">
         <v>14</v>
       </c>
-      <c r="CW8" t="s">
+      <c r="CX8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:101">
+    <row r="9" spans="1:102">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -3182,7 +3209,7 @@
         <v>38</v>
       </c>
       <c r="U9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="V9" t="s">
         <v>32</v>
@@ -3197,7 +3224,7 @@
         <v>60</v>
       </c>
       <c r="Z9" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="AA9" t="s">
         <v>67</v>
@@ -3296,7 +3323,7 @@
         <v>38</v>
       </c>
       <c r="BG9" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="BH9" t="s">
         <v>47</v>
@@ -3332,7 +3359,7 @@
         <v>30</v>
       </c>
       <c r="BS9" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="BT9" t="s">
         <v>12</v>
@@ -3359,7 +3386,7 @@
         <v>47</v>
       </c>
       <c r="CB9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="CC9" t="s">
         <v>44</v>
@@ -3389,7 +3416,7 @@
         <v>44</v>
       </c>
       <c r="CL9" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="CM9" t="s">
         <v>20</v>
@@ -3416,16 +3443,19 @@
         <v>77</v>
       </c>
       <c r="CU9" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="CV9" t="s">
+        <v>97</v>
+      </c>
+      <c r="CW9" t="s">
         <v>29</v>
       </c>
-      <c r="CW9" t="s">
+      <c r="CX9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:101">
+    <row r="10" spans="1:102">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3487,7 +3517,7 @@
         <v>57</v>
       </c>
       <c r="U10" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="V10" t="s">
         <v>29</v>
@@ -3502,7 +3532,7 @@
         <v>86</v>
       </c>
       <c r="Z10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="AA10" t="s">
         <v>81</v>
@@ -3601,7 +3631,7 @@
         <v>60</v>
       </c>
       <c r="BG10" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="BH10" t="s">
         <v>68</v>
@@ -3610,7 +3640,7 @@
         <v>24</v>
       </c>
       <c r="BJ10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BK10" t="s">
         <v>1</v>
@@ -3637,7 +3667,7 @@
         <v>81</v>
       </c>
       <c r="BS10" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="BT10" t="s">
         <v>23</v>
@@ -3658,7 +3688,7 @@
         <v>86</v>
       </c>
       <c r="BZ10" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="CA10" t="s">
         <v>68</v>
@@ -3694,7 +3724,7 @@
         <v>67</v>
       </c>
       <c r="CL10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="CM10" t="s">
         <v>39</v>
@@ -3721,16 +3751,19 @@
         <v>96</v>
       </c>
       <c r="CU10" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="CV10" t="s">
+        <v>77</v>
+      </c>
+      <c r="CW10" t="s">
         <v>63</v>
       </c>
-      <c r="CW10" t="s">
+      <c r="CX10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:101">
+    <row r="11" spans="1:102">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -3792,7 +3825,7 @@
         <v>34</v>
       </c>
       <c r="U11" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="V11" t="s">
         <v>28</v>
@@ -3807,7 +3840,7 @@
         <v>17</v>
       </c>
       <c r="Z11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AA11" t="s">
         <v>42</v>
@@ -3906,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="BG11" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="BH11" t="s">
         <v>95</v>
@@ -3942,7 +3975,7 @@
         <v>42</v>
       </c>
       <c r="BS11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="BT11" t="s">
         <v>65</v>
@@ -3963,7 +3996,7 @@
         <v>61</v>
       </c>
       <c r="BZ11" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="CA11" t="s">
         <v>74</v>
@@ -3999,7 +4032,7 @@
         <v>66</v>
       </c>
       <c r="CL11" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="CM11" t="s">
         <v>63</v>
@@ -4008,10 +4041,10 @@
         <v>96</v>
       </c>
       <c r="CO11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="CP11" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="CQ11" t="s">
         <v>62</v>
@@ -4026,16 +4059,19 @@
         <v>39</v>
       </c>
       <c r="CU11" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="CV11" t="s">
+        <v>84</v>
+      </c>
+      <c r="CW11" t="s">
         <v>21</v>
       </c>
-      <c r="CW11" t="s">
+      <c r="CX11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:101">
+    <row r="12" spans="1:102">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -4097,7 +4133,7 @@
         <v>51</v>
       </c>
       <c r="U12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="V12" t="s">
         <v>75</v>
@@ -4112,7 +4148,7 @@
         <v>34</v>
       </c>
       <c r="Z12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AA12" t="s">
         <v>72</v>
@@ -4202,7 +4238,7 @@
         <v>27</v>
       </c>
       <c r="BD12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BE12" t="s">
         <v>40</v>
@@ -4211,7 +4247,7 @@
         <v>12</v>
       </c>
       <c r="BG12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="BH12" t="s">
         <v>63</v>
@@ -4223,7 +4259,7 @@
         <v>51</v>
       </c>
       <c r="BK12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BL12" t="s">
         <v>68</v>
@@ -4247,7 +4283,7 @@
         <v>72</v>
       </c>
       <c r="BS12" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="BT12" t="s">
         <v>18</v>
@@ -4268,7 +4304,7 @@
         <v>51</v>
       </c>
       <c r="BZ12" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="CA12" t="s">
         <v>39</v>
@@ -4304,7 +4340,7 @@
         <v>81</v>
       </c>
       <c r="CL12" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="CM12" t="s">
         <v>51</v>
@@ -4313,10 +4349,10 @@
         <v>75</v>
       </c>
       <c r="CO12" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="CP12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="CQ12" t="s">
         <v>63</v>
@@ -4325,22 +4361,25 @@
         <v>83</v>
       </c>
       <c r="CS12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="CT12" t="s">
         <v>70</v>
       </c>
       <c r="CU12" t="s">
+        <v>43</v>
+      </c>
+      <c r="CV12" t="s">
         <v>53</v>
       </c>
-      <c r="CV12" t="s">
+      <c r="CW12" t="s">
         <v>91</v>
       </c>
-      <c r="CW12" t="s">
+      <c r="CX12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:101">
+    <row r="13" spans="1:102">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -4375,7 +4414,7 @@
         <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M13" t="s">
         <v>54</v>
@@ -4402,7 +4441,7 @@
         <v>5</v>
       </c>
       <c r="U13" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="V13" t="s">
         <v>33</v>
@@ -4417,7 +4456,7 @@
         <v>71</v>
       </c>
       <c r="Z13" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="AA13" t="s">
         <v>36</v>
@@ -4495,7 +4534,7 @@
         <v>35</v>
       </c>
       <c r="AZ13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BA13" t="s">
         <v>75</v>
@@ -4516,7 +4555,7 @@
         <v>48</v>
       </c>
       <c r="BG13" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="BH13" t="s">
         <v>29</v>
@@ -4552,7 +4591,7 @@
         <v>36</v>
       </c>
       <c r="BS13" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="BT13" t="s">
         <v>60</v>
@@ -4573,7 +4612,7 @@
         <v>38</v>
       </c>
       <c r="BZ13" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="CA13" t="s">
         <v>94</v>
@@ -4594,7 +4633,7 @@
         <v>29</v>
       </c>
       <c r="CG13" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="CH13" t="s">
         <v>35</v>
@@ -4609,19 +4648,19 @@
         <v>82</v>
       </c>
       <c r="CL13" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="CM13" t="s">
         <v>94</v>
       </c>
       <c r="CN13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="CO13" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="CP13" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="CQ13" t="s">
         <v>20</v>
@@ -4630,22 +4669,25 @@
         <v>3</v>
       </c>
       <c r="CS13" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="CT13" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="CU13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="CV13" t="s">
+        <v>96</v>
+      </c>
+      <c r="CW13" t="s">
         <v>87</v>
       </c>
-      <c r="CW13" t="s">
+      <c r="CX13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:101">
+    <row r="14" spans="1:102">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -4689,7 +4731,7 @@
         <v>38</v>
       </c>
       <c r="O14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P14" t="s">
         <v>80</v>
@@ -4707,7 +4749,7 @@
         <v>27</v>
       </c>
       <c r="U14" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="V14" t="s">
         <v>97</v>
@@ -4722,7 +4764,7 @@
         <v>57</v>
       </c>
       <c r="Z14" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="AA14" t="s">
         <v>35</v>
@@ -4821,7 +4863,7 @@
         <v>24</v>
       </c>
       <c r="BG14" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="BH14" t="s">
         <v>14</v>
@@ -4857,7 +4899,7 @@
         <v>80</v>
       </c>
       <c r="BS14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="BT14" t="s">
         <v>27</v>
@@ -4878,7 +4920,7 @@
         <v>5</v>
       </c>
       <c r="BZ14" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="CA14" t="s">
         <v>11</v>
@@ -4899,7 +4941,7 @@
         <v>11</v>
       </c>
       <c r="CG14" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="CH14" t="s">
         <v>80</v>
@@ -4908,13 +4950,13 @@
         <v>38</v>
       </c>
       <c r="CJ14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="CK14" t="s">
         <v>85</v>
       </c>
       <c r="CL14" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="CM14" t="s">
         <v>22</v>
@@ -4923,10 +4965,10 @@
         <v>3</v>
       </c>
       <c r="CO14" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="CP14" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="CQ14" t="s">
         <v>32</v>
@@ -4935,22 +4977,25 @@
         <v>52</v>
       </c>
       <c r="CS14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="CT14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="CU14" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="CV14" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW14" t="s">
         <v>8</v>
       </c>
-      <c r="CW14" t="s">
+      <c r="CX14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:101">
+    <row r="15" spans="1:102">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4973,7 +5018,7 @@
         <v>31</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I15" t="s">
         <v>68</v>
@@ -5012,7 +5057,7 @@
         <v>48</v>
       </c>
       <c r="U15" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="V15" t="s">
         <v>92</v>
@@ -5027,7 +5072,7 @@
         <v>31</v>
       </c>
       <c r="Z15" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="AA15" t="s">
         <v>88</v>
@@ -5108,7 +5153,7 @@
         <v>1</v>
       </c>
       <c r="BA15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BB15" t="s">
         <v>84</v>
@@ -5126,7 +5171,7 @@
         <v>10</v>
       </c>
       <c r="BG15" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="BH15" t="s">
         <v>33</v>
@@ -5162,7 +5207,7 @@
         <v>31</v>
       </c>
       <c r="BS15" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="BT15" t="s">
         <v>48</v>
@@ -5183,7 +5228,7 @@
         <v>34</v>
       </c>
       <c r="BZ15" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="CA15" t="s">
         <v>63</v>
@@ -5204,7 +5249,7 @@
         <v>39</v>
       </c>
       <c r="CG15" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="CH15" t="s">
         <v>88</v>
@@ -5219,7 +5264,7 @@
         <v>9</v>
       </c>
       <c r="CL15" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="CM15" t="s">
         <v>97</v>
@@ -5228,10 +5273,10 @@
         <v>32</v>
       </c>
       <c r="CO15" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="CP15" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="CQ15" t="s">
         <v>74</v>
@@ -5240,22 +5285,25 @@
         <v>33</v>
       </c>
       <c r="CS15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="CT15" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="CU15" t="s">
+        <v>97</v>
+      </c>
+      <c r="CV15" t="s">
         <v>28</v>
       </c>
-      <c r="CV15" t="s">
+      <c r="CW15" t="s">
         <v>68</v>
       </c>
-      <c r="CW15" t="s">
+      <c r="CX15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:101">
+    <row r="16" spans="1:102">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -5296,7 +5344,7 @@
         <v>5</v>
       </c>
       <c r="N16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O16" t="s">
         <v>53</v>
@@ -5317,7 +5365,7 @@
         <v>13</v>
       </c>
       <c r="U16" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="V16" t="s">
         <v>74</v>
@@ -5332,7 +5380,7 @@
         <v>1</v>
       </c>
       <c r="Z16" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="AA16" t="s">
         <v>80</v>
@@ -5341,7 +5389,7 @@
         <v>17</v>
       </c>
       <c r="AC16" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AD16" t="s">
         <v>53</v>
@@ -5395,7 +5443,7 @@
         <v>76</v>
       </c>
       <c r="AU16" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="AV16" t="s">
         <v>14</v>
@@ -5431,7 +5479,7 @@
         <v>19</v>
       </c>
       <c r="BG16" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="BH16" t="s">
         <v>21</v>
@@ -5467,7 +5515,7 @@
         <v>88</v>
       </c>
       <c r="BS16" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="BT16" t="s">
         <v>69</v>
@@ -5488,7 +5536,7 @@
         <v>57</v>
       </c>
       <c r="BZ16" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="CA16" t="s">
         <v>33</v>
@@ -5509,7 +5557,7 @@
         <v>28</v>
       </c>
       <c r="CG16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="CH16" t="s">
         <v>72</v>
@@ -5524,7 +5572,7 @@
         <v>69</v>
       </c>
       <c r="CL16" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="CM16" t="s">
         <v>28</v>
@@ -5533,10 +5581,10 @@
         <v>14</v>
       </c>
       <c r="CO16" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="CP16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="CQ16" t="s">
         <v>84</v>
@@ -5545,22 +5593,25 @@
         <v>21</v>
       </c>
       <c r="CS16" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="CT16" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="CU16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="CV16" t="s">
+        <v>62</v>
+      </c>
+      <c r="CW16" t="s">
         <v>53</v>
       </c>
-      <c r="CW16" t="s">
+      <c r="CX16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:101">
+    <row r="17" spans="1:102">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -5586,7 +5637,7 @@
         <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J17" t="s">
         <v>36</v>
@@ -5622,7 +5673,7 @@
         <v>60</v>
       </c>
       <c r="U17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="V17" t="s">
         <v>4</v>
@@ -5637,7 +5688,7 @@
         <v>5</v>
       </c>
       <c r="Z17" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="AA17" t="s">
         <v>40</v>
@@ -5646,7 +5697,7 @@
         <v>37</v>
       </c>
       <c r="AC17" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="AD17" t="s">
         <v>83</v>
@@ -5700,7 +5751,7 @@
         <v>23</v>
       </c>
       <c r="AU17" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="AV17" t="s">
         <v>21</v>
@@ -5736,7 +5787,7 @@
         <v>51</v>
       </c>
       <c r="BG17" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="BH17" t="s">
         <v>94</v>
@@ -5772,7 +5823,7 @@
         <v>71</v>
       </c>
       <c r="BS17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="BT17" t="s">
         <v>26</v>
@@ -5793,7 +5844,7 @@
         <v>48</v>
       </c>
       <c r="BZ17" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="CA17" t="s">
         <v>14</v>
@@ -5814,7 +5865,7 @@
         <v>63</v>
       </c>
       <c r="CG17" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="CH17" t="s">
         <v>36</v>
@@ -5829,7 +5880,7 @@
         <v>73</v>
       </c>
       <c r="CL17" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="CM17" t="s">
         <v>62</v>
@@ -5838,10 +5889,10 @@
         <v>53</v>
       </c>
       <c r="CO17" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="CP17" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="CQ17" t="s">
         <v>47</v>
@@ -5850,24 +5901,27 @@
         <v>91</v>
       </c>
       <c r="CS17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="CT17" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="CU17" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="CV17" t="s">
+        <v>46</v>
+      </c>
+      <c r="CW17" t="s">
         <v>96</v>
       </c>
-      <c r="CW17" t="s">
+      <c r="CX17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:101">
+    <row r="18" spans="1:102">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -5927,7 +5981,7 @@
         <v>55</v>
       </c>
       <c r="U18" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="V18" t="s">
         <v>87</v>
@@ -5942,7 +5996,7 @@
         <v>37</v>
       </c>
       <c r="Z18" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="AA18" t="s">
         <v>31</v>
@@ -5951,7 +6005,7 @@
         <v>10</v>
       </c>
       <c r="AC18" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="AD18" t="s">
         <v>96</v>
@@ -5966,7 +6020,7 @@
         <v>29</v>
       </c>
       <c r="AH18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AI18" t="s">
         <v>22</v>
@@ -6005,7 +6059,7 @@
         <v>12</v>
       </c>
       <c r="AU18" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="AV18" t="s">
         <v>11</v>
@@ -6026,7 +6080,7 @@
         <v>74</v>
       </c>
       <c r="BB18" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="BC18" t="s">
         <v>57</v>
@@ -6041,7 +6095,7 @@
         <v>22</v>
       </c>
       <c r="BG18" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="BH18" t="s">
         <v>11</v>
@@ -6077,7 +6131,7 @@
         <v>35</v>
       </c>
       <c r="BS18" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="BT18" t="s">
         <v>49</v>
@@ -6098,7 +6152,7 @@
         <v>22</v>
       </c>
       <c r="BZ18" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="CA18" t="s">
         <v>29</v>
@@ -6119,7 +6173,7 @@
         <v>95</v>
       </c>
       <c r="CG18" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="CH18" t="s">
         <v>81</v>
@@ -6134,7 +6188,7 @@
         <v>26</v>
       </c>
       <c r="CL18" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="CM18" t="s">
         <v>43</v>
@@ -6143,10 +6197,10 @@
         <v>74</v>
       </c>
       <c r="CO18" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="CP18" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="CQ18" t="s">
         <v>98</v>
@@ -6155,22 +6209,25 @@
         <v>29</v>
       </c>
       <c r="CS18" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="CT18" t="s">
+        <v>62</v>
+      </c>
+      <c r="CU18" t="s">
+        <v>94</v>
+      </c>
+      <c r="CV18" t="s">
+        <v>94</v>
+      </c>
+      <c r="CW18" t="s">
+        <v>47</v>
+      </c>
+      <c r="CX18" t="s">
         <v>98</v>
       </c>
-      <c r="CU18" t="s">
-        <v>39</v>
-      </c>
-      <c r="CV18" t="s">
-        <v>47</v>
-      </c>
-      <c r="CW18" t="s">
-        <v>98</v>
-      </c>
     </row>
-    <row r="19" spans="1:101">
+    <row r="19" spans="1:102">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -6232,7 +6289,7 @@
         <v>22</v>
       </c>
       <c r="U19" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="V19" t="s">
         <v>47</v>
@@ -6247,7 +6304,7 @@
         <v>42</v>
       </c>
       <c r="Z19" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="AA19" t="s">
         <v>71</v>
@@ -6256,10 +6313,10 @@
         <v>19</v>
       </c>
       <c r="AC19" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="AD19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AE19" t="s">
         <v>31</v>
@@ -6310,7 +6367,7 @@
         <v>7</v>
       </c>
       <c r="AU19" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="AV19" t="s">
         <v>29</v>
@@ -6331,7 +6388,7 @@
         <v>96</v>
       </c>
       <c r="BB19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="BC19" t="s">
         <v>86</v>
@@ -6346,7 +6403,7 @@
         <v>6</v>
       </c>
       <c r="BG19" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="BH19" t="s">
         <v>39</v>
@@ -6382,7 +6439,7 @@
         <v>40</v>
       </c>
       <c r="BS19" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="BT19" t="s">
         <v>1</v>
@@ -6403,7 +6460,7 @@
         <v>27</v>
       </c>
       <c r="BZ19" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="CA19" t="s">
         <v>28</v>
@@ -6424,7 +6481,7 @@
         <v>14</v>
       </c>
       <c r="CG19" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="CH19" t="s">
         <v>66</v>
@@ -6439,19 +6496,19 @@
         <v>49</v>
       </c>
       <c r="CL19" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="CM19" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="CN19" t="s">
         <v>4</v>
       </c>
       <c r="CO19" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="CP19" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="CQ19" t="s">
         <v>83</v>
@@ -6460,22 +6517,25 @@
         <v>94</v>
       </c>
       <c r="CS19" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="CT19" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="CU19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="CV19" t="s">
+        <v>93</v>
+      </c>
+      <c r="CW19" t="s">
         <v>74</v>
       </c>
-      <c r="CW19" t="s">
+      <c r="CX19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:101">
+    <row r="20" spans="1:102">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -6537,13 +6597,13 @@
         <v>12</v>
       </c>
       <c r="U20" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="V20" t="s">
         <v>83</v>
       </c>
       <c r="W20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="X20" t="s">
         <v>45</v>
@@ -6552,7 +6612,7 @@
         <v>10</v>
       </c>
       <c r="Z20" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="AA20" t="s">
         <v>54</v>
@@ -6561,7 +6621,7 @@
         <v>54</v>
       </c>
       <c r="AC20" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="AD20" t="s">
         <v>75</v>
@@ -6615,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="AU20" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="AV20" t="s">
         <v>94</v>
@@ -6636,7 +6696,7 @@
         <v>4</v>
       </c>
       <c r="BB20" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="BC20" t="s">
         <v>10</v>
@@ -6651,7 +6711,7 @@
         <v>37</v>
       </c>
       <c r="BG20" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="BH20" t="s">
         <v>52</v>
@@ -6687,7 +6747,7 @@
         <v>54</v>
       </c>
       <c r="BS20" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="BT20" t="s">
         <v>34</v>
@@ -6708,7 +6768,7 @@
         <v>43</v>
       </c>
       <c r="BZ20" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="CA20" t="s">
         <v>21</v>
@@ -6729,7 +6789,7 @@
         <v>33</v>
       </c>
       <c r="CG20" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="CH20" t="s">
         <v>67</v>
@@ -6744,19 +6804,19 @@
         <v>30</v>
       </c>
       <c r="CL20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="CM20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="CN20" t="s">
         <v>47</v>
       </c>
       <c r="CO20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="CP20" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="CQ20" t="s">
         <v>21</v>
@@ -6765,22 +6825,25 @@
         <v>39</v>
       </c>
       <c r="CS20" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="CT20" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="CU20" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="CV20" t="s">
+        <v>90</v>
+      </c>
+      <c r="CW20" t="s">
         <v>4</v>
       </c>
-      <c r="CW20" t="s">
+      <c r="CX20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:101">
+    <row r="21" spans="1:102">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -6842,7 +6905,7 @@
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="V21" t="s">
         <v>93</v>
@@ -6857,7 +6920,7 @@
         <v>45</v>
       </c>
       <c r="Z21" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AA21" t="s">
         <v>17</v>
@@ -6866,7 +6929,7 @@
         <v>22</v>
       </c>
       <c r="AC21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AD21" t="s">
         <v>32</v>
@@ -6920,7 +6983,7 @@
         <v>10</v>
       </c>
       <c r="AU21" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AV21" t="s">
         <v>53</v>
@@ -6941,7 +7004,7 @@
         <v>59</v>
       </c>
       <c r="BB21" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="BC21" t="s">
         <v>26</v>
@@ -6956,7 +7019,7 @@
         <v>17</v>
       </c>
       <c r="BG21" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="BH21" t="s">
         <v>28</v>
@@ -6992,7 +7055,7 @@
         <v>17</v>
       </c>
       <c r="BS21" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="BT21" t="s">
         <v>57</v>
@@ -7013,7 +7076,7 @@
         <v>60</v>
       </c>
       <c r="BZ21" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="CA21" t="s">
         <v>52</v>
@@ -7034,7 +7097,7 @@
         <v>91</v>
       </c>
       <c r="CG21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="CH21" t="s">
         <v>30</v>
@@ -7049,19 +7112,19 @@
         <v>64</v>
       </c>
       <c r="CL21" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="CM21" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="CN21" t="s">
         <v>28</v>
       </c>
       <c r="CO21" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="CP21" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="CQ21" t="s">
         <v>89</v>
@@ -7070,18 +7133,21 @@
         <v>28</v>
       </c>
       <c r="CS21" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="CT21" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="CU21" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="CV21" t="s">
+        <v>101</v>
+      </c>
+      <c r="CW21" t="s">
         <v>28</v>
       </c>
-      <c r="CW21" t="s">
+      <c r="CX21" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>